<commit_message>
Fix typo in test file
</commit_message>
<xml_diff>
--- a/tests/FsSpreadsheet.ExcelIO.Tests/data/testUnit.xlsx
+++ b/tests/FsSpreadsheet.ExcelIO.Tests/data/testUnit.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muehl\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\CSBiology\FsSpreadsheet\tests\FsSpreadsheet.ExcelIO.Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC4075A-BA46-47DE-B230-29A9E1DCD683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBC93C7-A01E-493F-9D50-85997A5A5958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="3840" windowWidth="18810" windowHeight="15370" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StringSheet" sheetId="1" r:id="rId1"/>
     <sheet name="NumericSheet" sheetId="2" r:id="rId2"/>
-    <sheet name="TabelSheet" sheetId="3" r:id="rId3"/>
+    <sheet name="TableSheet" sheetId="3" r:id="rId3"/>
     <sheet name="DataTypeSheet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -220,7 +220,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -513,13 +513,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -547,7 +545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -561,7 +559,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -575,7 +573,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -589,7 +587,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -603,7 +601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -617,7 +615,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -631,7 +629,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -645,7 +643,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -659,7 +657,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -673,7 +671,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -695,12 +693,12 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -714,7 +712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -728,7 +726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -742,7 +740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -756,7 +754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -770,7 +768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -784,7 +782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -798,7 +796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -812,7 +810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -826,7 +824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -840,7 +838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -854,7 +852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -874,13 +872,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FABCFE-B3AE-4047-B3ED-254CF2AB7F9A}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -894,7 +892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -908,7 +906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -922,7 +920,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -936,7 +934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -950,7 +948,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -964,7 +962,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -978,7 +976,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -992,7 +990,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1006,7 +1004,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1020,7 +1018,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1034,7 +1032,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1058,31 +1056,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E6D016-A7BF-4D1C-82FF-984F9E9E846D}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>3.14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Update test Xlsx file
</commit_message>
<xml_diff>
--- a/tests/FsSpreadsheet.ExcelIO.Tests/data/testUnit.xlsx
+++ b/tests/FsSpreadsheet.ExcelIO.Tests/data/testUnit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\CSBiology\FsSpreadsheet\tests\FsSpreadsheet.ExcelIO.Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBC93C7-A01E-493F-9D50-85997A5A5958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11078C7A-0BFD-4324-A370-A0665F857FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StringSheet" sheetId="1" r:id="rId1"/>
@@ -213,11 +213,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -692,179 +693,187 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF703C5D-67D2-43D2-90AF-7DCAB03188F0}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="4">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="4">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="4">
         <v>1</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>6</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>7</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>8</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>9</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>10</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>12</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>12</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4">
         <v>13</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -872,7 +881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FABCFE-B3AE-4047-B3ED-254CF2AB7F9A}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>